<commit_message>
complete read data from excel for 3 test cases in ViewListProducts
</commit_message>
<xml_diff>
--- a/test cases/DienmayXANH-ViewListProducts.xlsx
+++ b/test cases/DienmayXANH-ViewListProducts.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\eclipse-workspace\DienMayXanh\test cases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\eclipse-workspace\DienmayXANH\DienMayXanh\test cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88CB2CBB-D974-4620-B3C4-ED1792366111}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD48ACA0-130B-47B0-B9AF-8C750E471198}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1654,10 +1654,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.6640625" customWidth="1"/>
-    <col min="3" max="3" width="14.44140625" customWidth="1"/>
-    <col min="4" max="4" width="30.33203125" customWidth="1"/>
-    <col min="5" max="5" width="53.5546875" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.44140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="30.33203125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="53.5546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:5" ht="21" x14ac:dyDescent="0.3">
@@ -1848,12 +1848,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" customWidth="1"/>
-    <col min="2" max="2" width="16.109375" customWidth="1"/>
-    <col min="3" max="3" width="28.44140625" customWidth="1"/>
-    <col min="4" max="4" width="38.6640625" customWidth="1"/>
-    <col min="5" max="5" width="13.109375" customWidth="1"/>
-    <col min="6" max="6" width="13.88671875" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28.44140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="38.6640625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.109375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.88671875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -2074,20 +2074,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="22.88671875" customWidth="1"/>
-    <col min="3" max="3" width="21.33203125" customWidth="1"/>
-    <col min="4" max="4" width="28.21875" customWidth="1"/>
-    <col min="5" max="5" width="16.44140625" customWidth="1"/>
-    <col min="6" max="6" width="8.33203125" customWidth="1"/>
-    <col min="7" max="7" width="31.33203125" style="27" customWidth="1"/>
-    <col min="8" max="8" width="19.6640625" customWidth="1"/>
-    <col min="9" max="9" width="36.109375" style="27" customWidth="1"/>
+    <col min="2" max="2" width="22.88671875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21.33203125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="28.21875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.44140625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="8.33203125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="31.33203125" style="27" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="19.6640625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="36.109375" style="27" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.6">

</xml_diff>